<commit_message>
Edited the entire code to only use RNA abundances to check for presence while pulling relative abundances from the DNA data set. Re-did the classifications. There was error in the previous version where DNA data set was also being used to check for active otus which was fixed in this version. All OTUs were reclassified correctly as (persistent,seasonal,transient) based on the RNA data set. This version is error free and we will be pivoting to this version for further analysis and manuscript.
</commit_message>
<xml_diff>
--- a/rna.persistent.classified.timeseries.aquatic.otus.rna.present.atl.once.xlsx
+++ b/rna.persistent.classified.timeseries.aquatic.otus.rna.present.atl.once.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,7 +432,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Otu00015</t>
+          <t>Otu00017</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -444,7 +444,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Otu00016</t>
+          <t>Otu00020</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -456,7 +456,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Otu00017</t>
+          <t>Otu00024</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -468,7 +468,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Otu00020</t>
+          <t>Otu00029</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -480,7 +480,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Otu00029</t>
+          <t>Otu00034</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -492,7 +492,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Otu00034</t>
+          <t>Otu00038</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -504,7 +504,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Otu00037</t>
+          <t>Otu00047</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -516,7 +516,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Otu00038</t>
+          <t>Otu00056</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -528,7 +528,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Otu00047</t>
+          <t>Otu00062</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -540,7 +540,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Otu00076</t>
+          <t>Otu00067</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -552,10 +552,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Otu00123</t>
+          <t>Otu00073</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
+        <is>
+          <t>persistent</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Otu00219</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>persistent</t>
         </is>

</xml_diff>